<commit_message>
Test case file created
V1, more to do
</commit_message>
<xml_diff>
--- a/Getting a loan/Account.xlsx
+++ b/Getting a loan/Account.xlsx
@@ -62,7 +62,7 @@
     <x:t>Current</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> 75909</x:t>
+    <x:t xml:space="preserve"> 70891</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -522,7 +522,7 @@
     <x:row r="28" spans="1:7" x14ac:dyDescent="0.3"/>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" r:id="rId5"/>
+    <x:hyperlink ref="B2" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>